<commit_message>
Order_Type Exceptions added to excel
</commit_message>
<xml_diff>
--- a/GE3_TestCasesTemplate_2023_v1.0.xlsx
+++ b/GE3_TestCasesTemplate_2023_v1.0.xlsx
@@ -1,14 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED2E733-8416-4DB0-A64F-CE04843CF782}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="11010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="GE3 2023 F1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="GE3 2023 F2" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="GE3 2023 F3" sheetId="3" r:id="rId6"/>
+    <sheet name="GE3 2023 F1" sheetId="1" r:id="rId1"/>
+    <sheet name="GE3 2023 F2" sheetId="2" r:id="rId2"/>
+    <sheet name="GE3 2023 F3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mimM9jobA4i0ITBU4OLLvFuneX8gw=="/>
@@ -18,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="61">
   <si>
     <t>#</t>
   </si>
@@ -98,9 +107,6 @@
     <t>CE_NV_2</t>
   </si>
   <si>
-    <t>PRODUCT ID NOT NUMBER</t>
-  </si>
-  <si>
     <t>842169142322A</t>
   </si>
   <si>
@@ -114,24 +120,6 @@
   </si>
   <si>
     <t>PRODUCT ID NOT CHECK SUM</t>
-  </si>
-  <si>
-    <t>CE_V_8</t>
-  </si>
-  <si>
-    <t>ecc7f631f98930aca6e183c6e505dFFF</t>
-  </si>
-  <si>
-    <t>CE_NV_9</t>
-  </si>
-  <si>
-    <t>ORDER_TYPE WRONG</t>
-  </si>
-  <si>
-    <t>"PRE"</t>
-  </si>
-  <si>
-    <t>Exception : order type wrong</t>
   </si>
   <si>
     <t>OUTPUT</t>
@@ -201,70 +189,108 @@
   <si>
     <t>Path considering that the input is not found in the file</t>
   </si>
+  <si>
+    <t>"regular"</t>
+  </si>
+  <si>
+    <t>"Premium"</t>
+  </si>
+  <si>
+    <t>"premiums"</t>
+  </si>
+  <si>
+    <t>PRODUCT ID NOT (EA13)NUMBER</t>
+  </si>
+  <si>
+    <t>"regula"</t>
+  </si>
+  <si>
+    <t>Exception: Order Type not valid</t>
+  </si>
+  <si>
+    <t>ORDER_TYPE NOT VALID (not a string)</t>
+  </si>
+  <si>
+    <t>ORDER_TYPE NOT VALID (not equal to either of the valid options(tto few))</t>
+  </si>
+  <si>
+    <t>ORDER_TYPE NOT VALID (not equal to either of the valid options(too much))</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="12">
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="12"/>
       <color rgb="FF067D17"/>
       <name val="JetBrains Mono"/>
     </font>
     <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="0"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="12"/>
       <color theme="0"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF067D17"/>
+      <name val="JetBrains Mono"/>
     </font>
   </fonts>
   <fills count="4">
@@ -272,7 +298,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -288,169 +314,203 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+  <cellXfs count="18">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="9">
     <dxf>
-      <font/>
       <fill>
-        <patternFill patternType="none"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E2F3"/>
+          <bgColor rgb="FFD9E2F3"/>
+        </patternFill>
       </fill>
-      <border/>
     </dxf>
     <dxf>
-      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E2F3"/>
+          <bgColor rgb="FFD9E2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="4"/>
           <bgColor theme="4"/>
         </patternFill>
       </fill>
-      <border/>
     </dxf>
     <dxf>
-      <font/>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFD9E2F3"/>
           <bgColor rgb="FFD9E2F3"/>
         </patternFill>
       </fill>
-      <border/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E2F3"/>
+          <bgColor rgb="FFD9E2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E2F3"/>
+          <bgColor rgb="FFD9E2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E2F3"/>
+          <bgColor rgb="FFD9E2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="3">
-    <tableStyle count="3" pivot="0" name="GE3 2023 F1-style">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="2" type="secondRowStripe"/>
+    <tableStyle name="GE3 2023 F1-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="headerRow" dxfId="8"/>
+      <tableStyleElement type="firstRowStripe" dxfId="7"/>
+      <tableStyleElement type="secondRowStripe" dxfId="6"/>
     </tableStyle>
-    <tableStyle count="3" pivot="0" name="GE3 2023 F2-style">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="2" type="secondRowStripe"/>
+    <tableStyle name="GE3 2023 F2-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
+      <tableStyleElement type="headerRow" dxfId="5"/>
+      <tableStyleElement type="firstRowStripe" dxfId="4"/>
+      <tableStyleElement type="secondRowStripe" dxfId="3"/>
     </tableStyle>
-    <tableStyle count="3" pivot="0" name="GE3 2023 F3-style">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="2" type="secondRowStripe"/>
+    <tableStyle name="GE3 2023 F3-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
+      <tableStyleElement type="headerRow" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="secondRowStripe" dxfId="0"/>
     </tableStyle>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:N44" displayName="Table_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:N44">
   <tableColumns count="14">
-    <tableColumn name="#" id="1"/>
-    <tableColumn name="I/O" id="2"/>
-    <tableColumn name="TECHNIQUE" id="3"/>
-    <tableColumn name="FIELD" id="4"/>
-    <tableColumn name="VALID/INVALID" id="5"/>
-    <tableColumn name="ID TEST" id="6"/>
-    <tableColumn name="DESCRIPTION" id="7"/>
-    <tableColumn name="PRODUCT_ID" id="8"/>
-    <tableColumn name="ORDER_TYPE" id="9"/>
-    <tableColumn name="ADDRESS" id="10"/>
-    <tableColumn name="PHONE_NUMBER" id="11"/>
-    <tableColumn name="ZIP_CODE" id="12"/>
-    <tableColumn name="RESULT" id="13"/>
-    <tableColumn name="OBSERVATIONS" id="14"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="#"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="I/O"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="TECHNIQUE"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="FIELD"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="VALID/INVALID"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="ID TEST"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="DESCRIPTION"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="PRODUCT_ID"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="ORDER_TYPE"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="ADDRESS"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="PHONE_NUMBER"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="ZIP_CODE"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="RESULT"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="OBSERVATIONS"/>
   </tableColumns>
-  <tableStyleInfo name="GE3 2023 F1-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="GE3 2023 F1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:J43" displayName="Table_2" id="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_2" displayName="Table_2" ref="A1:J43">
   <tableColumns count="10">
-    <tableColumn name="#" id="1"/>
-    <tableColumn name="NODE" id="2"/>
-    <tableColumn name="TERMINAL  (T) / NO TERMINAL (NT)" id="3"/>
-    <tableColumn name="TYPE (DUPLICATION / DELETION / MODIFICATION / VALID)" id="4"/>
-    <tableColumn name="ID TEST" id="5"/>
-    <tableColumn name="DESCRIPTION" id="6"/>
-    <tableColumn name="FILE PATH" id="7"/>
-    <tableColumn name="FILE CONTENT" id="8"/>
-    <tableColumn name="EXPECTED RESULT" id="9"/>
-    <tableColumn name="OBSERVATIONS" id="10"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="#"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="NODE"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="TERMINAL  (T) / NO TERMINAL (NT)"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="TYPE (DUPLICATION / DELETION / MODIFICATION / VALID)"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="ID TEST"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="DESCRIPTION"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="FILE PATH"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="FILE CONTENT"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="EXPECTED RESULT"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="OBSERVATIONS"/>
   </tableColumns>
-  <tableStyleInfo name="GE3 2023 F2-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="GE3 2023 F2-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G43" displayName="Table_3" id="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table_3" displayName="Table_3" ref="A1:G43">
   <tableColumns count="7">
-    <tableColumn name="#" id="1"/>
-    <tableColumn name="PATH" id="2"/>
-    <tableColumn name="ID TEST" id="3"/>
-    <tableColumn name="DESCRIPTION" id="4"/>
-    <tableColumn name="KEY" id="5"/>
-    <tableColumn name="EXPECTED RESULT" id="6"/>
-    <tableColumn name="OBSERVATIONS" id="7"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="#"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="PATH"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="ID TEST"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="DESCRIPTION"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="KEY"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="EXPECTED RESULT"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="OBSERVATIONS"/>
   </tableColumns>
-  <tableStyleInfo name="GE3 2023 F3-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="GE3 2023 F3-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -640,35 +700,37 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AD1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11:J13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="10.1" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.109375" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="10.6"/>
-    <col customWidth="1" min="3" max="3" width="8.5"/>
-    <col customWidth="1" min="4" max="4" width="14.3"/>
-    <col customWidth="1" min="5" max="5" width="11.3"/>
-    <col customWidth="1" min="6" max="6" width="14.8"/>
-    <col customWidth="1" min="7" max="7" width="22.2"/>
-    <col customWidth="1" min="8" max="8" width="18.1"/>
-    <col customWidth="1" min="9" max="9" width="14.0"/>
-    <col customWidth="1" min="10" max="10" width="31.3"/>
-    <col customWidth="1" min="11" max="11" width="14.2"/>
-    <col customWidth="1" min="12" max="12" width="13.3"/>
-    <col customWidth="1" min="13" max="13" width="70.9"/>
-    <col customWidth="1" min="14" max="30" width="10.6"/>
+    <col min="1" max="2" width="10.609375" customWidth="1"/>
+    <col min="3" max="3" width="8.5" customWidth="1"/>
+    <col min="4" max="4" width="14.27734375" customWidth="1"/>
+    <col min="5" max="5" width="11.27734375" customWidth="1"/>
+    <col min="6" max="6" width="14.77734375" customWidth="1"/>
+    <col min="7" max="7" width="22.21875" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="31.27734375" customWidth="1"/>
+    <col min="11" max="11" width="14.21875" customWidth="1"/>
+    <col min="12" max="12" width="13.27734375" customWidth="1"/>
+    <col min="13" max="13" width="70.88671875" customWidth="1"/>
+    <col min="14" max="30" width="10.609375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:30" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -728,9 +790,9 @@
       <c r="AC1" s="4"/>
       <c r="AD1" s="4"/>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:30" ht="15.75" customHeight="1">
       <c r="A2" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>14</v>
@@ -751,7 +813,7 @@
         <v>18</v>
       </c>
       <c r="H2" s="8">
-        <v>8.42169142322E12</v>
+        <v>8421691423220</v>
       </c>
       <c r="I2" s="8" t="s">
         <v>19</v>
@@ -770,9 +832,9 @@
       </c>
       <c r="N2" s="5"/>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:30" ht="15.75" customHeight="1">
       <c r="A3" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>14</v>
@@ -790,13 +852,13 @@
         <v>25</v>
       </c>
       <c r="G3" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="I3" s="9" t="s">
         <v>27</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>28</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>20</v>
@@ -808,13 +870,13 @@
         <v>22</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N3" s="5"/>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:30" ht="15.75" customHeight="1">
       <c r="A4" s="5">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>14</v>
@@ -829,13 +891,13 @@
         <v>24</v>
       </c>
       <c r="F4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>31</v>
-      </c>
       <c r="H4" s="9">
-        <v>8.421691423225E12</v>
+        <v>8421691423225</v>
       </c>
       <c r="I4" s="8" t="s">
         <v>19</v>
@@ -850,18 +912,24 @@
         <v>22</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N4" s="5"/>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:30" ht="15.75" customHeight="1">
       <c r="A5" s="5">
-        <v>4.0</v>
-      </c>
-      <c r="B5" s="6"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="C5" s="6"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="6"/>
+      <c r="D5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="8"/>
@@ -872,69 +940,97 @@
       <c r="M5" s="9"/>
       <c r="N5" s="5"/>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:30" ht="15.75" customHeight="1">
       <c r="A6" s="5">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
+      <c r="D6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="8"/>
+      <c r="G6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="8">
+        <v>8421691423220</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="N6" s="5"/>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:30" ht="15.75" customHeight="1">
       <c r="A7" s="5">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
+      <c r="D7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="8"/>
+      <c r="G7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="8">
+        <v>8421691423220</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="N7" s="5"/>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="5">
-        <v>7.0</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>15</v>
-      </c>
+    <row r="8" spans="1:30" ht="15.75" customHeight="1">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
       <c r="D8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>32</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="7"/>
       <c r="G8" s="7" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="H8" s="8">
-        <v>8.42169142322E12</v>
+        <v>8421691423220</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>20</v>
@@ -942,41 +1038,33 @@
       <c r="K8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="L8" s="10" t="s">
+      <c r="L8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="M8" s="9" t="s">
-        <v>33</v>
+      <c r="M8" s="8" t="s">
+        <v>57</v>
       </c>
       <c r="N8" s="5"/>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="5">
-        <v>8.0</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>15</v>
-      </c>
+    <row r="9" spans="1:30" ht="15.75" customHeight="1">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
       <c r="D9" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>35</v>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7" t="s">
+        <v>58</v>
       </c>
       <c r="H9" s="8">
-        <v>8.42169142322E12</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>36</v>
+        <v>8421691423220</v>
+      </c>
+      <c r="I9" s="9">
+        <v>123</v>
       </c>
       <c r="J9" s="9" t="s">
         <v>20</v>
@@ -984,94 +1072,116 @@
       <c r="K9" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="L9" s="10" t="s">
+      <c r="L9" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="M9" s="9" t="s">
-        <v>37</v>
+      <c r="M9" s="8" t="s">
+        <v>57</v>
       </c>
       <c r="N9" s="5"/>
     </row>
-    <row r="10" ht="16.5" customHeight="1">
-      <c r="A10" s="5">
-        <v>9.0</v>
-      </c>
+    <row r="10" spans="1:30" ht="15.75" customHeight="1">
+      <c r="A10" s="5"/>
       <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="8"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" s="8">
+        <v>8421691423220</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" s="8" t="s">
+        <v>57</v>
+      </c>
       <c r="N10" s="5"/>
     </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="5">
-        <v>10.0</v>
-      </c>
+    <row r="11" spans="1:30" ht="15.75" customHeight="1">
+      <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
+      <c r="D11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="12"/>
       <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="17"/>
       <c r="K11" s="8"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="8"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="9"/>
       <c r="N11" s="5"/>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="5">
-        <v>11.0</v>
-      </c>
+    <row r="12" spans="1:30" ht="15.75" customHeight="1">
+      <c r="A12" s="5"/>
       <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
       <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="17"/>
       <c r="K12" s="8"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="8"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="9"/>
       <c r="N12" s="5"/>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="5">
-        <v>12.0</v>
-      </c>
+    <row r="13" spans="1:30" ht="15.75" customHeight="1">
+      <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="7"/>
+      <c r="G13" s="12"/>
       <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="17"/>
       <c r="K13" s="8"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="8"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="9"/>
       <c r="N13" s="5"/>
     </row>
-    <row r="14" ht="15.75" customHeight="1">
+    <row r="14" spans="1:30" ht="15.75" customHeight="1">
       <c r="A14" s="5">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+      <c r="E14" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="8"/>
@@ -1082,14 +1192,16 @@
       <c r="M14" s="8"/>
       <c r="N14" s="5"/>
     </row>
-    <row r="15" ht="15.75" customHeight="1">
+    <row r="15" spans="1:30" ht="15.75" customHeight="1">
       <c r="A15" s="5">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="E15" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="8"/>
@@ -1100,14 +1212,16 @@
       <c r="M15" s="8"/>
       <c r="N15" s="5"/>
     </row>
-    <row r="16" ht="15.75" customHeight="1">
+    <row r="16" spans="1:30" ht="15.75" customHeight="1">
       <c r="A16" s="5">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="E16" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="8"/>
@@ -1118,12 +1232,14 @@
       <c r="M16" s="8"/>
       <c r="N16" s="5"/>
     </row>
-    <row r="17" ht="15.75" customHeight="1">
+    <row r="17" spans="1:14" ht="15.75" customHeight="1">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+      <c r="E17" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="8"/>
@@ -1134,7 +1250,7 @@
       <c r="M17" s="8"/>
       <c r="N17" s="5"/>
     </row>
-    <row r="18" ht="15.75" customHeight="1">
+    <row r="18" spans="1:14" ht="15.75" customHeight="1">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -1150,9 +1266,9 @@
       <c r="M18" s="8"/>
       <c r="N18" s="5"/>
     </row>
-    <row r="19" ht="15.75" customHeight="1">
+    <row r="19" spans="1:14" ht="15.75" customHeight="1">
       <c r="A19" s="5">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -1168,9 +1284,9 @@
       <c r="M19" s="8"/>
       <c r="N19" s="5"/>
     </row>
-    <row r="20" ht="15.75" customHeight="1">
+    <row r="20" spans="1:14" ht="15.75" customHeight="1">
       <c r="A20" s="5">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -1186,9 +1302,9 @@
       <c r="M20" s="8"/>
       <c r="N20" s="5"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
+    <row r="21" spans="1:14" ht="15.75" customHeight="1">
       <c r="A21" s="5">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -1204,9 +1320,9 @@
       <c r="M21" s="8"/>
       <c r="N21" s="5"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
+    <row r="22" spans="1:14" ht="15.75" customHeight="1">
       <c r="A22" s="5">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -1222,9 +1338,9 @@
       <c r="M22" s="8"/>
       <c r="N22" s="5"/>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
+    <row r="23" spans="1:14" ht="15.75" customHeight="1">
       <c r="A23" s="5">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
@@ -1240,9 +1356,9 @@
       <c r="M23" s="8"/>
       <c r="N23" s="5"/>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
+    <row r="24" spans="1:14" ht="15.75" customHeight="1">
       <c r="A24" s="5">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -1258,9 +1374,9 @@
       <c r="M24" s="8"/>
       <c r="N24" s="5"/>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
+    <row r="25" spans="1:14" ht="15.75" customHeight="1">
       <c r="A25" s="5">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -1276,9 +1392,9 @@
       <c r="M25" s="8"/>
       <c r="N25" s="5"/>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
+    <row r="26" spans="1:14" ht="15.75" customHeight="1">
       <c r="A26" s="5">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -1294,9 +1410,9 @@
       <c r="M26" s="8"/>
       <c r="N26" s="5"/>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
+    <row r="27" spans="1:14" ht="15.75" customHeight="1">
       <c r="A27" s="5">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -1312,9 +1428,9 @@
       <c r="M27" s="8"/>
       <c r="N27" s="8"/>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
+    <row r="28" spans="1:14" ht="15.75" customHeight="1">
       <c r="A28" s="5">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -1330,9 +1446,9 @@
       <c r="M28" s="8"/>
       <c r="N28" s="5"/>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
+    <row r="29" spans="1:14" ht="15.75" customHeight="1">
       <c r="A29" s="5">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -1348,9 +1464,9 @@
       <c r="M29" s="8"/>
       <c r="N29" s="5"/>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
+    <row r="30" spans="1:14" ht="15.75" customHeight="1">
       <c r="A30" s="5">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -1366,9 +1482,9 @@
       <c r="M30" s="8"/>
       <c r="N30" s="5"/>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
+    <row r="31" spans="1:14" ht="15.75" customHeight="1">
       <c r="A31" s="5">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -1384,9 +1500,9 @@
       <c r="M31" s="8"/>
       <c r="N31" s="5"/>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
+    <row r="32" spans="1:14" ht="15.75" customHeight="1">
       <c r="A32" s="5">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -1402,9 +1518,9 @@
       <c r="M32" s="5"/>
       <c r="N32" s="5"/>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
+    <row r="33" spans="1:14" ht="15.75" customHeight="1">
       <c r="A33" s="5">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -1420,23 +1536,23 @@
       <c r="M33" s="5"/>
       <c r="N33" s="5"/>
     </row>
-    <row r="34" ht="15.75" customHeight="1">
+    <row r="34" spans="1:14" ht="15.75" customHeight="1">
       <c r="A34" s="5">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F34" s="5"/>
       <c r="G34" s="5" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
@@ -1446,23 +1562,23 @@
       <c r="M34" s="5"/>
       <c r="N34" s="5"/>
     </row>
-    <row r="35" ht="15.75" customHeight="1">
+    <row r="35" spans="1:14" ht="15.75" customHeight="1">
       <c r="A35" s="5">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="5" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="F35" s="5"/>
       <c r="G35" s="5" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
@@ -1472,7 +1588,7 @@
       <c r="M35" s="5"/>
       <c r="N35" s="5"/>
     </row>
-    <row r="36" ht="15.75" customHeight="1">
+    <row r="36" spans="1:14" ht="15.75" customHeight="1">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -1488,7 +1604,7 @@
       <c r="M36" s="5"/>
       <c r="N36" s="5"/>
     </row>
-    <row r="37" ht="15.75" customHeight="1">
+    <row r="37" spans="1:14" ht="15.75" customHeight="1">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -1504,7 +1620,7 @@
       <c r="M37" s="5"/>
       <c r="N37" s="5"/>
     </row>
-    <row r="38" ht="15.75" customHeight="1">
+    <row r="38" spans="1:14" ht="15.75" customHeight="1">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -1520,7 +1636,7 @@
       <c r="M38" s="5"/>
       <c r="N38" s="5"/>
     </row>
-    <row r="39" ht="15.75" customHeight="1">
+    <row r="39" spans="1:14" ht="15.75" customHeight="1">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -1536,7 +1652,7 @@
       <c r="M39" s="5"/>
       <c r="N39" s="5"/>
     </row>
-    <row r="40" ht="15.75" customHeight="1">
+    <row r="40" spans="1:14" ht="15.75" customHeight="1">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -1552,7 +1668,7 @@
       <c r="M40" s="5"/>
       <c r="N40" s="5"/>
     </row>
-    <row r="41" ht="15.75" customHeight="1">
+    <row r="41" spans="1:14" ht="15.75" customHeight="1">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -1568,7 +1684,7 @@
       <c r="M41" s="5"/>
       <c r="N41" s="5"/>
     </row>
-    <row r="42" ht="15.75" customHeight="1">
+    <row r="42" spans="1:14" ht="15.75" customHeight="1">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -1584,7 +1700,7 @@
       <c r="M42" s="5"/>
       <c r="N42" s="5"/>
     </row>
-    <row r="43" ht="15.75" customHeight="1">
+    <row r="43" spans="1:14" ht="15.75" customHeight="1">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -1600,7 +1716,7 @@
       <c r="M43" s="5"/>
       <c r="N43" s="5"/>
     </row>
-    <row r="44" ht="15.75" customHeight="1">
+    <row r="44" spans="1:14" ht="15.75" customHeight="1">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
@@ -1616,10 +1732,10 @@
       <c r="M44" s="5"/>
       <c r="N44" s="5"/>
     </row>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
+    <row r="45" spans="1:14" ht="15.75" customHeight="1"/>
+    <row r="46" spans="1:14" ht="15.75" customHeight="1"/>
+    <row r="47" spans="1:14" ht="15.75" customHeight="1"/>
+    <row r="48" spans="1:14" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>
@@ -2574,49 +2690,45 @@
     <row r="1000" ht="15.75" customHeight="1"/>
     <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AB1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="10.1" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.109375" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="10.6"/>
-    <col customWidth="1" min="3" max="3" width="26.6"/>
-    <col customWidth="1" min="4" max="4" width="44.1"/>
-    <col customWidth="1" min="5" max="5" width="22.3"/>
-    <col customWidth="1" min="6" max="6" width="62.3"/>
-    <col customWidth="1" min="7" max="7" width="9.3"/>
-    <col customWidth="1" min="8" max="8" width="36.7"/>
-    <col customWidth="1" min="9" max="10" width="33.7"/>
-    <col customWidth="1" min="11" max="28" width="10.6"/>
+    <col min="1" max="2" width="10.609375" customWidth="1"/>
+    <col min="3" max="3" width="26.609375" customWidth="1"/>
+    <col min="4" max="4" width="44.109375" customWidth="1"/>
+    <col min="5" max="5" width="22.27734375" customWidth="1"/>
+    <col min="6" max="6" width="62.27734375" customWidth="1"/>
+    <col min="7" max="7" width="9.27734375" customWidth="1"/>
+    <col min="8" max="8" width="36.71875" customWidth="1"/>
+    <col min="9" max="10" width="33.71875" customWidth="1"/>
+    <col min="11" max="28" width="10.609375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="33.0" customHeight="1">
+    <row r="1" spans="1:28" ht="33" customHeight="1">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>5</v>
@@ -2625,13 +2737,13 @@
         <v>6</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="J1" s="15" t="s">
         <v>13</v>
@@ -2655,39 +2767,39 @@
       <c r="AA1" s="16"/>
       <c r="AB1" s="16"/>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:28" ht="15.75" customHeight="1">
       <c r="A2" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="5">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:28" ht="15.75" customHeight="1">
       <c r="A3" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -2699,9 +2811,9 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:28" ht="15.75" customHeight="1">
       <c r="A4" s="5">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -2713,9 +2825,9 @@
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:28" ht="15.75" customHeight="1">
       <c r="A5" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -2727,9 +2839,9 @@
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:28" ht="15.75" customHeight="1">
       <c r="A6" s="5">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -2741,7 +2853,7 @@
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:28" ht="15.75" customHeight="1">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -2753,7 +2865,7 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
+    <row r="8" spans="1:28" ht="15.75" customHeight="1">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -2765,7 +2877,7 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
+    <row r="9" spans="1:28" ht="15.75" customHeight="1">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -2777,7 +2889,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" ht="15.75" customHeight="1">
+    <row r="10" spans="1:28" ht="15.75" customHeight="1">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -2789,7 +2901,7 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" ht="15.75" customHeight="1">
+    <row r="11" spans="1:28" ht="15.75" customHeight="1">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -2801,7 +2913,7 @@
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
+    <row r="12" spans="1:28" ht="15.75" customHeight="1">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -2813,7 +2925,7 @@
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
+    <row r="13" spans="1:28" ht="15.75" customHeight="1">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -2825,7 +2937,7 @@
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" ht="15.75" customHeight="1">
+    <row r="14" spans="1:28" ht="15.75" customHeight="1">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -2837,7 +2949,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" ht="15.75" customHeight="1">
+    <row r="15" spans="1:28" ht="15.75" customHeight="1">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -2849,7 +2961,7 @@
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" ht="15.75" customHeight="1">
+    <row r="16" spans="1:28" ht="15.75" customHeight="1">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -2861,7 +2973,7 @@
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" ht="15.75" customHeight="1">
+    <row r="17" spans="1:10" ht="15.75" customHeight="1">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -2873,7 +2985,7 @@
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" ht="15.75" customHeight="1">
+    <row r="18" spans="1:10" ht="15.75" customHeight="1">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -2885,7 +2997,7 @@
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" ht="15.75" customHeight="1">
+    <row r="19" spans="1:10" ht="15.75" customHeight="1">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -2897,7 +3009,7 @@
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" ht="15.75" customHeight="1">
+    <row r="20" spans="1:10" ht="15.75" customHeight="1">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -2909,7 +3021,7 @@
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
+    <row r="21" spans="1:10" ht="15.75" customHeight="1">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -2921,7 +3033,7 @@
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
+    <row r="22" spans="1:10" ht="15.75" customHeight="1">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -2933,7 +3045,7 @@
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
+    <row r="23" spans="1:10" ht="15.75" customHeight="1">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -2945,7 +3057,7 @@
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
+    <row r="24" spans="1:10" ht="15.75" customHeight="1">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -2957,7 +3069,7 @@
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
+    <row r="25" spans="1:10" ht="15.75" customHeight="1">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -2969,7 +3081,7 @@
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
+    <row r="26" spans="1:10" ht="15.75" customHeight="1">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -2981,7 +3093,7 @@
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
+    <row r="27" spans="1:10" ht="15.75" customHeight="1">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -2993,7 +3105,7 @@
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
+    <row r="28" spans="1:10" ht="15.75" customHeight="1">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -3005,7 +3117,7 @@
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
+    <row r="29" spans="1:10" ht="15.75" customHeight="1">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -3017,7 +3129,7 @@
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
+    <row r="30" spans="1:10" ht="15.75" customHeight="1">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -3029,7 +3141,7 @@
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
+    <row r="31" spans="1:10" ht="15.75" customHeight="1">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -3041,7 +3153,7 @@
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
+    <row r="32" spans="1:10" ht="15.75" customHeight="1">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -3053,7 +3165,7 @@
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
+    <row r="33" spans="1:10" ht="15.75" customHeight="1">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -3065,7 +3177,7 @@
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" ht="15.75" customHeight="1">
+    <row r="34" spans="1:10" ht="15.75" customHeight="1">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -3077,7 +3189,7 @@
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
     </row>
-    <row r="35" ht="15.75" customHeight="1">
+    <row r="35" spans="1:10" ht="15.75" customHeight="1">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -3089,7 +3201,7 @@
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
     </row>
-    <row r="36" ht="15.75" customHeight="1">
+    <row r="36" spans="1:10" ht="15.75" customHeight="1">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -3101,7 +3213,7 @@
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
     </row>
-    <row r="37" ht="15.75" customHeight="1">
+    <row r="37" spans="1:10" ht="15.75" customHeight="1">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -3113,7 +3225,7 @@
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
     </row>
-    <row r="38" ht="15.75" customHeight="1">
+    <row r="38" spans="1:10" ht="15.75" customHeight="1">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -3125,7 +3237,7 @@
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
     </row>
-    <row r="39" ht="15.75" customHeight="1">
+    <row r="39" spans="1:10" ht="15.75" customHeight="1">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -3137,7 +3249,7 @@
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
     </row>
-    <row r="40" ht="15.75" customHeight="1">
+    <row r="40" spans="1:10" ht="15.75" customHeight="1">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -3149,7 +3261,7 @@
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
     </row>
-    <row r="41" ht="15.75" customHeight="1">
+    <row r="41" spans="1:10" ht="15.75" customHeight="1">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -3161,7 +3273,7 @@
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
     </row>
-    <row r="42" ht="15.75" customHeight="1">
+    <row r="42" spans="1:10" ht="15.75" customHeight="1">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -3173,7 +3285,7 @@
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
     </row>
-    <row r="43" ht="15.75" customHeight="1">
+    <row r="43" spans="1:10" ht="15.75" customHeight="1">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -3185,11 +3297,11 @@
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
     </row>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
+    <row r="44" spans="1:10" ht="15.75" customHeight="1"/>
+    <row r="45" spans="1:10" ht="15.75" customHeight="1"/>
+    <row r="46" spans="1:10" ht="15.75" customHeight="1"/>
+    <row r="47" spans="1:10" ht="15.75" customHeight="1"/>
+    <row r="48" spans="1:10" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>
@@ -4143,41 +4255,37 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="10.1" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.109375" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="10.6"/>
-    <col customWidth="1" min="2" max="2" width="15.6"/>
-    <col customWidth="1" min="3" max="3" width="22.3"/>
-    <col customWidth="1" min="4" max="4" width="62.3"/>
-    <col customWidth="1" min="5" max="5" width="9.3"/>
-    <col customWidth="1" min="6" max="7" width="33.7"/>
-    <col customWidth="1" min="8" max="25" width="10.6"/>
+    <col min="1" max="1" width="10.609375" customWidth="1"/>
+    <col min="2" max="2" width="15.609375" customWidth="1"/>
+    <col min="3" max="3" width="22.27734375" customWidth="1"/>
+    <col min="4" max="4" width="62.27734375" customWidth="1"/>
+    <col min="5" max="5" width="9.27734375" customWidth="1"/>
+    <col min="6" max="7" width="33.71875" customWidth="1"/>
+    <col min="8" max="25" width="10.609375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>5</v>
@@ -4186,33 +4294,33 @@
         <v>6</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -4221,9 +4329,9 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="5">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -4232,9 +4340,9 @@
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -4243,9 +4351,9 @@
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="5">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -4254,7 +4362,7 @@
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -4263,7 +4371,7 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -4272,7 +4380,7 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -4281,7 +4389,7 @@
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" ht="15.75" customHeight="1">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -4290,7 +4398,7 @@
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" ht="15.75" customHeight="1">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -4299,7 +4407,7 @@
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -4308,7 +4416,7 @@
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -4317,7 +4425,7 @@
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" ht="15.75" customHeight="1">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -4326,7 +4434,7 @@
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" ht="15.75" customHeight="1">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -4335,7 +4443,7 @@
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" ht="15.75" customHeight="1">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -4344,7 +4452,7 @@
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" ht="15.75" customHeight="1">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -4353,7 +4461,7 @@
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" ht="15.75" customHeight="1">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -4362,7 +4470,7 @@
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" ht="15.75" customHeight="1">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -4371,7 +4479,7 @@
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" ht="15.75" customHeight="1">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -4380,7 +4488,7 @@
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -4389,7 +4497,7 @@
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -4398,7 +4506,7 @@
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -4407,7 +4515,7 @@
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -4416,7 +4524,7 @@
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -4425,7 +4533,7 @@
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -4434,7 +4542,7 @@
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -4443,7 +4551,7 @@
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
+    <row r="28" spans="1:7" ht="15.75" customHeight="1">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -4452,7 +4560,7 @@
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
+    <row r="29" spans="1:7" ht="15.75" customHeight="1">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -4461,7 +4569,7 @@
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
+    <row r="30" spans="1:7" ht="15.75" customHeight="1">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -4470,7 +4578,7 @@
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
+    <row r="31" spans="1:7" ht="15.75" customHeight="1">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -4479,7 +4587,7 @@
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
+    <row r="32" spans="1:7" ht="15.75" customHeight="1">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -4488,7 +4596,7 @@
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
+    <row r="33" spans="1:7" ht="15.75" customHeight="1">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -4497,7 +4605,7 @@
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
     </row>
-    <row r="34" ht="15.75" customHeight="1">
+    <row r="34" spans="1:7" ht="15.75" customHeight="1">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -4506,7 +4614,7 @@
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
     </row>
-    <row r="35" ht="15.75" customHeight="1">
+    <row r="35" spans="1:7" ht="15.75" customHeight="1">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -4515,7 +4623,7 @@
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
     </row>
-    <row r="36" ht="15.75" customHeight="1">
+    <row r="36" spans="1:7" ht="15.75" customHeight="1">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -4524,7 +4632,7 @@
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
     </row>
-    <row r="37" ht="15.75" customHeight="1">
+    <row r="37" spans="1:7" ht="15.75" customHeight="1">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -4533,7 +4641,7 @@
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
     </row>
-    <row r="38" ht="15.75" customHeight="1">
+    <row r="38" spans="1:7" ht="15.75" customHeight="1">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -4542,7 +4650,7 @@
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
     </row>
-    <row r="39" ht="15.75" customHeight="1">
+    <row r="39" spans="1:7" ht="15.75" customHeight="1">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -4551,7 +4659,7 @@
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
     </row>
-    <row r="40" ht="15.75" customHeight="1">
+    <row r="40" spans="1:7" ht="15.75" customHeight="1">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -4560,7 +4668,7 @@
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
     </row>
-    <row r="41" ht="15.75" customHeight="1">
+    <row r="41" spans="1:7" ht="15.75" customHeight="1">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -4569,7 +4677,7 @@
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
     </row>
-    <row r="42" ht="15.75" customHeight="1">
+    <row r="42" spans="1:7" ht="15.75" customHeight="1">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -4578,7 +4686,7 @@
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
     </row>
-    <row r="43" ht="15.75" customHeight="1">
+    <row r="43" spans="1:7" ht="15.75" customHeight="1">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -4587,11 +4695,11 @@
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
     </row>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
+    <row r="44" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="45" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="46" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="47" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="48" spans="1:7" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>
@@ -5545,12 +5653,10 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added test cases for Phone Number
</commit_message>
<xml_diff>
--- a/GE3_TestCasesTemplate_2023_v1.0.xlsx
+++ b/GE3_TestCasesTemplate_2023_v1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edu/PycharmProjects/G89.2023.T20.EG3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390B2950-A83C-CA49-BF00-8B703F7875C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B7850DF-50F0-584B-B071-4A01B45CDC1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="900" yWindow="500" windowWidth="27900" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GE3 2023 F1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="101">
   <si>
     <t>#</t>
   </si>
@@ -211,12 +211,6 @@
     <t>ORDER_TYPE NOT VALID (not a string)</t>
   </si>
   <si>
-    <t>ORDER_TYPE NOT VALID (not equal to either of the valid options(tto few))</t>
-  </si>
-  <si>
-    <t>ORDER_TYPE NOT VALID (not equal to either of the valid options(too much))</t>
-  </si>
-  <si>
     <t>ADDRES</t>
   </si>
   <si>
@@ -266,13 +260,88 @@
   </si>
   <si>
     <t>Exception: Address too long</t>
+  </si>
+  <si>
+    <t>CE_NV_4</t>
+  </si>
+  <si>
+    <t>CE_NV_8</t>
+  </si>
+  <si>
+    <t>CE_NV_9</t>
+  </si>
+  <si>
+    <t>CE_NV_10</t>
+  </si>
+  <si>
+    <t>CE_V_5</t>
+  </si>
+  <si>
+    <t>CE_V_6</t>
+  </si>
+  <si>
+    <t>PHONE_NUMBER_TYPE NOT VALID</t>
+  </si>
+  <si>
+    <t>ORDER_TYPE NOT VALID TOO LONG</t>
+  </si>
+  <si>
+    <t>ORDER_TYPE NOT VALID TOO SHORT</t>
+  </si>
+  <si>
+    <t>CE_V_17</t>
+  </si>
+  <si>
+    <t>"DEATH_STAR"</t>
+  </si>
+  <si>
+    <t>Exception: Phone_number is not a number</t>
+  </si>
+  <si>
+    <t>"123456789"</t>
+  </si>
+  <si>
+    <t>CE_NV_18</t>
+  </si>
+  <si>
+    <t>VALD</t>
+  </si>
+  <si>
+    <t>CE_V_19</t>
+  </si>
+  <si>
+    <t>PHONE_NUMBER VALID</t>
+  </si>
+  <si>
+    <t>¿Valid Phone number?</t>
+  </si>
+  <si>
+    <t>CE_NV_XX</t>
+  </si>
+  <si>
+    <t>PHONE_NUMBER TOO SHORT</t>
+  </si>
+  <si>
+    <t>"123456"</t>
+  </si>
+  <si>
+    <t>Exception: Phone_number too short</t>
+  </si>
+  <si>
+    <t>PHONE_NUMBER TOO LONG</t>
+  </si>
+  <si>
+    <t>"123456789123456"</t>
+  </si>
+  <si>
+    <t>Exception: Phone_number too long</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -346,8 +415,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF008000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -366,6 +447,12 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -379,7 +466,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -394,10 +481,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="11" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -759,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:M15"/>
+    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.140625" defaultRowHeight="15" customHeight="1"/>
@@ -770,7 +862,7 @@
     <col min="4" max="4" width="14.28515625" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" customWidth="1"/>
+    <col min="7" max="7" width="30.28515625" customWidth="1"/>
     <col min="8" max="8" width="18.140625" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
     <col min="10" max="10" width="31.28515625" customWidth="1"/>
@@ -872,9 +964,9 @@
         <v>20</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="L2" s="13" t="s">
         <v>22</v>
       </c>
       <c r="M2" s="6" t="s">
@@ -916,7 +1008,7 @@
       <c r="K3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="13" t="s">
         <v>22</v>
       </c>
       <c r="M3" s="6" t="s">
@@ -958,7 +1050,7 @@
       <c r="K4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="L4" s="13" t="s">
         <v>22</v>
       </c>
       <c r="M4" s="6" t="s">
@@ -973,20 +1065,24 @@
       <c r="B5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="D5" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="5"/>
+      <c r="F5" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="G5" s="5"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
-      <c r="L5" s="7"/>
+      <c r="L5" s="13"/>
       <c r="M5" s="6"/>
       <c r="N5" s="4"/>
     </row>
@@ -994,15 +1090,21 @@
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
+      <c r="B6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="D6" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="5"/>
+      <c r="F6" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="G6" s="5" t="s">
         <v>18</v>
       </c>
@@ -1018,7 +1120,7 @@
       <c r="K6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="L6" s="13" t="s">
         <v>22</v>
       </c>
       <c r="M6" s="6" t="s">
@@ -1030,15 +1132,21 @@
       <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+      <c r="B7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="D7" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="5"/>
+      <c r="F7" s="5" t="s">
+        <v>81</v>
+      </c>
       <c r="G7" s="5" t="s">
         <v>18</v>
       </c>
@@ -1054,7 +1162,7 @@
       <c r="K7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="L7" s="13" t="s">
         <v>22</v>
       </c>
       <c r="M7" s="6" t="s">
@@ -1063,18 +1171,26 @@
       <c r="N7" s="4"/>
     </row>
     <row r="8" spans="1:30" ht="15.75" customHeight="1">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5"/>
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="D8" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="5"/>
+      <c r="F8" s="5" t="s">
+        <v>77</v>
+      </c>
       <c r="G8" s="5" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="H8" s="6">
         <v>8421691423220</v>
@@ -1088,7 +1204,7 @@
       <c r="K8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L8" s="7" t="s">
+      <c r="L8" s="13" t="s">
         <v>22</v>
       </c>
       <c r="M8" s="6" t="s">
@@ -1097,16 +1213,24 @@
       <c r="N8" s="4"/>
     </row>
     <row r="9" spans="1:30" ht="15.75" customHeight="1">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="D9" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="5"/>
+      <c r="F9" s="5" t="s">
+        <v>78</v>
+      </c>
       <c r="G9" s="5" t="s">
         <v>58</v>
       </c>
@@ -1122,7 +1246,7 @@
       <c r="K9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L9" s="7" t="s">
+      <c r="L9" s="13" t="s">
         <v>22</v>
       </c>
       <c r="M9" s="6" t="s">
@@ -1131,18 +1255,26 @@
       <c r="N9" s="4"/>
     </row>
     <row r="10" spans="1:30" ht="15.75" customHeight="1">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="5"/>
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="D10" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="5" t="s">
+        <v>79</v>
+      </c>
       <c r="G10" s="5" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="H10" s="6">
         <v>8421691423220</v>
@@ -1156,7 +1288,7 @@
       <c r="K10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L10" s="7" t="s">
+      <c r="L10" s="13" t="s">
         <v>22</v>
       </c>
       <c r="M10" s="6" t="s">
@@ -1165,7 +1297,9 @@
       <c r="N10" s="4"/>
     </row>
     <row r="11" spans="1:30" ht="15.75" customHeight="1">
-      <c r="A11" s="4"/>
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
       <c r="B11" s="5" t="s">
         <v>14</v>
       </c>
@@ -1173,18 +1307,18 @@
         <v>15</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>16</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="6">
         <v>8421690000000</v>
       </c>
       <c r="I11" s="6" t="s">
@@ -1196,14 +1330,16 @@
       <c r="K11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L11" s="7" t="s">
+      <c r="L11" s="13" t="s">
         <v>22</v>
       </c>
       <c r="M11" s="6"/>
       <c r="N11" s="4"/>
     </row>
     <row r="12" spans="1:30" ht="15.75" customHeight="1">
-      <c r="A12" s="4"/>
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
       <c r="B12" s="5" t="s">
         <v>14</v>
       </c>
@@ -1211,39 +1347,41 @@
         <v>15</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>24</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H12" s="12">
+        <v>62</v>
+      </c>
+      <c r="H12" s="6">
         <v>8421690000000</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>19</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L12" s="7" t="s">
+      <c r="L12" s="13" t="s">
         <v>22</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N12" s="4"/>
     </row>
     <row r="13" spans="1:30" ht="15.75" customHeight="1">
-      <c r="A13" s="4"/>
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
       <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
@@ -1251,18 +1389,18 @@
         <v>15</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>24</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="H13" s="12">
+        <v>66</v>
+      </c>
+      <c r="H13" s="6">
         <v>8421690000000</v>
       </c>
       <c r="I13" s="6" t="s">
@@ -1274,11 +1412,11 @@
       <c r="K13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L13" s="7" t="s">
+      <c r="L13" s="13" t="s">
         <v>22</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N13" s="4"/>
     </row>
@@ -1293,34 +1431,34 @@
         <v>15</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>24</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="H14" s="12">
+        <v>69</v>
+      </c>
+      <c r="H14" s="6">
         <v>8421690000000</v>
       </c>
       <c r="I14" s="6" t="s">
         <v>19</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K14" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L14" s="7" t="s">
+      <c r="L14" s="13" t="s">
         <v>22</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="N14" s="4"/>
     </row>
@@ -1335,34 +1473,34 @@
         <v>15</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>24</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="H15" s="12">
+        <v>73</v>
+      </c>
+      <c r="H15" s="6">
         <v>8421690000000</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J15" s="13" t="s">
-        <v>76</v>
+      <c r="J15" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="K15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L15" s="7" t="s">
+      <c r="L15" s="13" t="s">
         <v>22</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="N15" s="4"/>
     </row>
@@ -1370,90 +1508,200 @@
       <c r="A16" s="4">
         <v>15</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="5" t="s">
+      <c r="B16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="6"/>
+      <c r="F16" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="14">
+        <v>8421690000000</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="J16" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="M16" s="15" t="s">
+        <v>23</v>
+      </c>
       <c r="N16" s="4"/>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1">
       <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="5" t="s">
+      <c r="B17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="6"/>
+      <c r="F17" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H17" s="14">
+        <v>8421690000000</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="J17" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K17" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="L17" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="M17" s="15" t="s">
+        <v>87</v>
+      </c>
       <c r="N17" s="4"/>
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1">
       <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
+      <c r="B18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H18" s="14">
+        <v>8421690000000</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="J18" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K18" s="15" t="s">
+        <v>88</v>
+      </c>
       <c r="L18" s="4"/>
-      <c r="M18" s="6"/>
+      <c r="M18" s="15" t="s">
+        <v>93</v>
+      </c>
       <c r="N18" s="4"/>
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1">
       <c r="A19" s="4">
         <v>16</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
+      <c r="B19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H19" s="14">
+        <v>8421690000000</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="J19" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K19" s="15" t="s">
+        <v>96</v>
+      </c>
       <c r="L19" s="4"/>
-      <c r="M19" s="6"/>
+      <c r="M19" s="15" t="s">
+        <v>97</v>
+      </c>
       <c r="N19" s="4"/>
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1">
       <c r="A20" s="4">
         <v>17</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
+      <c r="B20" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H20" s="14">
+        <v>8421690000000</v>
+      </c>
+      <c r="I20" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="J20" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K20" s="15" t="s">
+        <v>99</v>
+      </c>
       <c r="L20" s="4"/>
-      <c r="M20" s="6"/>
+      <c r="M20" s="15" t="s">
+        <v>100</v>
+      </c>
       <c r="N20" s="4"/>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1">
@@ -1466,12 +1714,18 @@
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
+      <c r="H21" s="14">
+        <v>8421690000000</v>
+      </c>
+      <c r="I21" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="J21" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K21" s="15"/>
       <c r="L21" s="4"/>
-      <c r="M21" s="6"/>
+      <c r="M21" s="16"/>
       <c r="N21" s="4"/>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1">
@@ -2856,7 +3110,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="165" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>

</xml_diff>

<commit_message>
New changes as pull does not work
</commit_message>
<xml_diff>
--- a/GE3_TestCasesTemplate_2023_v1.0.xlsx
+++ b/GE3_TestCasesTemplate_2023_v1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edu/PycharmProjects/G89.2023.T20.EG3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B7850DF-50F0-584B-B071-4A01B45CDC1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B18603B4-5DAE-AD4B-A260-4F8A5E958D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="900" yWindow="500" windowWidth="27900" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="101">
   <si>
     <t>#</t>
   </si>
@@ -466,7 +466,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -481,15 +481,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="11" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -851,8 +848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:M21"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.140625" defaultRowHeight="15" customHeight="1"/>
@@ -966,7 +963,7 @@
       <c r="K2" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="12" t="s">
         <v>22</v>
       </c>
       <c r="M2" s="6" t="s">
@@ -1008,7 +1005,7 @@
       <c r="K3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="L3" s="12" t="s">
         <v>22</v>
       </c>
       <c r="M3" s="6" t="s">
@@ -1050,7 +1047,7 @@
       <c r="K4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="13" t="s">
+      <c r="L4" s="12" t="s">
         <v>22</v>
       </c>
       <c r="M4" s="6" t="s">
@@ -1082,7 +1079,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
-      <c r="L5" s="13"/>
+      <c r="L5" s="12"/>
       <c r="M5" s="6"/>
       <c r="N5" s="4"/>
     </row>
@@ -1120,7 +1117,7 @@
       <c r="K6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L6" s="13" t="s">
+      <c r="L6" s="12" t="s">
         <v>22</v>
       </c>
       <c r="M6" s="6" t="s">
@@ -1162,7 +1159,7 @@
       <c r="K7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L7" s="13" t="s">
+      <c r="L7" s="12" t="s">
         <v>22</v>
       </c>
       <c r="M7" s="6" t="s">
@@ -1204,7 +1201,7 @@
       <c r="K8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L8" s="13" t="s">
+      <c r="L8" s="12" t="s">
         <v>22</v>
       </c>
       <c r="M8" s="6" t="s">
@@ -1246,7 +1243,7 @@
       <c r="K9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L9" s="13" t="s">
+      <c r="L9" s="12" t="s">
         <v>22</v>
       </c>
       <c r="M9" s="6" t="s">
@@ -1288,7 +1285,7 @@
       <c r="K10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L10" s="13" t="s">
+      <c r="L10" s="12" t="s">
         <v>22</v>
       </c>
       <c r="M10" s="6" t="s">
@@ -1330,7 +1327,7 @@
       <c r="K11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L11" s="13" t="s">
+      <c r="L11" s="12" t="s">
         <v>22</v>
       </c>
       <c r="M11" s="6"/>
@@ -1370,7 +1367,7 @@
       <c r="K12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L12" s="13" t="s">
+      <c r="L12" s="12" t="s">
         <v>22</v>
       </c>
       <c r="M12" s="6" t="s">
@@ -1412,7 +1409,7 @@
       <c r="K13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L13" s="13" t="s">
+      <c r="L13" s="12" t="s">
         <v>22</v>
       </c>
       <c r="M13" s="6" t="s">
@@ -1454,7 +1451,7 @@
       <c r="K14" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L14" s="13" t="s">
+      <c r="L14" s="12" t="s">
         <v>22</v>
       </c>
       <c r="M14" s="6" t="s">
@@ -1490,13 +1487,13 @@
       <c r="I15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J15" s="12" t="s">
+      <c r="J15" s="6" t="s">
         <v>74</v>
       </c>
       <c r="K15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L15" s="13" t="s">
+      <c r="L15" s="12" t="s">
         <v>22</v>
       </c>
       <c r="M15" s="6" t="s">
@@ -1526,22 +1523,22 @@
       <c r="G16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="14">
+      <c r="H16" s="6">
         <v>8421690000000</v>
       </c>
-      <c r="I16" s="15" t="s">
+      <c r="I16" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="J16" s="15" t="s">
+      <c r="J16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K16" s="15" t="s">
+      <c r="K16" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L16" s="15" t="s">
+      <c r="L16" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="M16" s="15" t="s">
+      <c r="M16" s="13" t="s">
         <v>23</v>
       </c>
       <c r="N16" s="4"/>
@@ -1566,22 +1563,22 @@
       <c r="G17" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="H17" s="14">
+      <c r="H17" s="6">
         <v>8421690000000</v>
       </c>
-      <c r="I17" s="15" t="s">
+      <c r="I17" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="J17" s="15" t="s">
+      <c r="J17" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K17" s="15" t="s">
+      <c r="K17" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="L17" s="15" t="s">
+      <c r="L17" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="M17" s="15" t="s">
+      <c r="M17" s="13" t="s">
         <v>87</v>
       </c>
       <c r="N17" s="4"/>
@@ -1606,20 +1603,20 @@
       <c r="G18" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H18" s="14">
+      <c r="H18" s="6">
         <v>8421690000000</v>
       </c>
-      <c r="I18" s="15" t="s">
+      <c r="I18" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="J18" s="15" t="s">
+      <c r="J18" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K18" s="15" t="s">
+      <c r="K18" s="6" t="s">
         <v>88</v>
       </c>
       <c r="L18" s="4"/>
-      <c r="M18" s="15" t="s">
+      <c r="M18" s="13" t="s">
         <v>93</v>
       </c>
       <c r="N18" s="4"/>
@@ -1646,20 +1643,20 @@
       <c r="G19" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="H19" s="14">
+      <c r="H19" s="6">
         <v>8421690000000</v>
       </c>
-      <c r="I19" s="15" t="s">
+      <c r="I19" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="J19" s="15" t="s">
+      <c r="J19" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K19" s="15" t="s">
+      <c r="K19" s="6" t="s">
         <v>96</v>
       </c>
       <c r="L19" s="4"/>
-      <c r="M19" s="15" t="s">
+      <c r="M19" s="13" t="s">
         <v>97</v>
       </c>
       <c r="N19" s="4"/>
@@ -1686,20 +1683,20 @@
       <c r="G20" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="H20" s="14">
+      <c r="H20" s="6">
         <v>8421690000000</v>
       </c>
-      <c r="I20" s="15" t="s">
+      <c r="I20" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="J20" s="15" t="s">
+      <c r="J20" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K20" s="15" t="s">
+      <c r="K20" s="6" t="s">
         <v>99</v>
       </c>
       <c r="L20" s="4"/>
-      <c r="M20" s="15" t="s">
+      <c r="M20" s="13" t="s">
         <v>100</v>
       </c>
       <c r="N20" s="4"/>
@@ -1714,18 +1711,12 @@
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
-      <c r="H21" s="14">
-        <v>8421690000000</v>
-      </c>
-      <c r="I21" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="J21" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K21" s="15"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
       <c r="L21" s="4"/>
-      <c r="M21" s="16"/>
+      <c r="M21" s="14"/>
       <c r="N21" s="4"/>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1">
@@ -1834,7 +1825,7 @@
       <c r="K27" s="6"/>
       <c r="L27" s="4"/>
       <c r="M27" s="6"/>
-      <c r="N27" s="6"/>
+      <c r="N27" s="15"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1">
       <c r="A28" s="4">

</xml_diff>

<commit_message>
Files from the last class (08-03-23)
</commit_message>
<xml_diff>
--- a/GE3_TestCasesTemplate_2023_v1.0.xlsx
+++ b/GE3_TestCasesTemplate_2023_v1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edu/PycharmProjects/G89.2023.T20.EG3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7039B089-C12F-4948-984A-614E7FA358A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BF027B-8B96-F840-AF60-898CB82C904A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="128">
   <si>
     <t>#</t>
   </si>
@@ -93,9 +93,6 @@
   </si>
   <si>
     <t>"28005"</t>
-  </si>
-  <si>
-    <t>ecc7f631f98930aca6e183c6e505dc45</t>
   </si>
   <si>
     <t>NOT VALID</t>
@@ -298,9 +295,6 @@
     <t>CE_NV_18</t>
   </si>
   <si>
-    <t>VALD</t>
-  </si>
-  <si>
     <t>CE_V_19</t>
   </si>
   <si>
@@ -310,9 +304,6 @@
     <t>¿Valid Phone number?</t>
   </si>
   <si>
-    <t>CE_NV_XX</t>
-  </si>
-  <si>
     <t>PHONE_NUMBER TOO SHORT</t>
   </si>
   <si>
@@ -392,13 +383,46 @@
   </si>
   <si>
     <t>"654314159"</t>
+  </si>
+  <si>
+    <t>abed71d395e4a85c2606d6e5d3a3579a</t>
+  </si>
+  <si>
+    <t>CE_NV_20</t>
+  </si>
+  <si>
+    <t>CE_NV_21</t>
+  </si>
+  <si>
+    <t>CE_NV_22</t>
+  </si>
+  <si>
+    <t>CE_V_23</t>
+  </si>
+  <si>
+    <t>CE_NV_24</t>
+  </si>
+  <si>
+    <t>CE_NV_25</t>
+  </si>
+  <si>
+    <t>CE_NV_26</t>
+  </si>
+  <si>
+    <t>CE_NV_27</t>
+  </si>
+  <si>
+    <t>CE_NV_28</t>
+  </si>
+  <si>
+    <t>"8421691423220"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -449,13 +473,6 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -535,7 +552,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -543,21 +560,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -919,8 +935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="116" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="116" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.140625" defaultRowHeight="15" customHeight="1"/>
@@ -1022,8 +1038,8 @@
       <c r="G2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="6">
-        <v>8421691423220</v>
+      <c r="H2" s="15" t="s">
+        <v>127</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>19</v>
@@ -1032,13 +1048,13 @@
         <v>20</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="L2" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="L2" s="12" t="s">
         <v>21</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>22</v>
+        <v>117</v>
       </c>
       <c r="N2" s="4"/>
     </row>
@@ -1056,31 +1072,31 @@
         <v>7</v>
       </c>
       <c r="E3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="H3" s="7" t="s">
+      <c r="I3" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>26</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="L3" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="L3" s="12" t="s">
         <v>21</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N3" s="4"/>
     </row>
@@ -1098,15 +1114,15 @@
         <v>7</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="6">
+      <c r="H4" s="15">
         <v>8421691423225</v>
       </c>
       <c r="I4" s="6" t="s">
@@ -1116,13 +1132,13 @@
         <v>20</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="L4" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="L4" s="12" t="s">
         <v>21</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N4" s="4"/>
     </row>
@@ -1140,19 +1156,19 @@
         <v>7</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G5" s="5"/>
-      <c r="H5" s="6"/>
+      <c r="H5" s="15"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="L5" s="15"/>
+        <v>116</v>
+      </c>
+      <c r="L5" s="12"/>
       <c r="M5" s="6"/>
       <c r="N5" s="4"/>
     </row>
@@ -1167,35 +1183,33 @@
         <v>15</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="15">
         <v>8421691423220</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="L6" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="L6" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="M6" s="6" t="s">
-        <v>22</v>
-      </c>
+      <c r="M6" s="6"/>
       <c r="N6" s="4"/>
     </row>
     <row r="7" spans="1:30" ht="15.75" customHeight="1">
@@ -1209,35 +1223,33 @@
         <v>15</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>16</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="15">
         <v>8421691423220</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="L7" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="L7" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="M7" s="6" t="s">
-        <v>22</v>
-      </c>
+      <c r="M7" s="6"/>
       <c r="N7" s="4"/>
     </row>
     <row r="8" spans="1:30" ht="15.75" customHeight="1">
@@ -1251,34 +1263,34 @@
         <v>15</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="H8" s="6">
+        <v>80</v>
+      </c>
+      <c r="H8" s="15">
         <v>8421691423220</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="L8" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="L8" s="12" t="s">
         <v>21</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="N8" s="4"/>
     </row>
@@ -1293,18 +1305,18 @@
         <v>15</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="H9" s="6">
+        <v>55</v>
+      </c>
+      <c r="H9" s="15">
         <v>8421691423220</v>
       </c>
       <c r="I9" s="6">
@@ -1314,13 +1326,13 @@
         <v>20</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="L9" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="L9" s="12" t="s">
         <v>21</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="N9" s="4"/>
     </row>
@@ -1335,34 +1347,34 @@
         <v>15</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="H10" s="6">
+        <v>81</v>
+      </c>
+      <c r="H10" s="15">
         <v>8421691423220</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J10" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="L10" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="L10" s="12" t="s">
         <v>21</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="N10" s="4"/>
     </row>
@@ -1377,19 +1389,19 @@
         <v>15</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>16</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="6">
-        <v>8421690000000</v>
+      <c r="H11" s="15">
+        <v>8421691423220</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>19</v>
@@ -1398,13 +1410,13 @@
         <v>20</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="L11" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="L11" s="12" t="s">
         <v>21</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>22</v>
+        <v>117</v>
       </c>
       <c r="N11" s="4"/>
     </row>
@@ -1419,34 +1431,34 @@
         <v>15</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F12" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="G12" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="H12" s="6">
-        <v>8421690000000</v>
+      <c r="H12" s="15">
+        <v>8421691423220</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>19</v>
       </c>
       <c r="J12" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="M12" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="L12" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="M12" s="6" t="s">
-        <v>62</v>
       </c>
       <c r="N12" s="4"/>
     </row>
@@ -1461,19 +1473,19 @@
         <v>15</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F13" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H13" s="6">
-        <v>8421690000000</v>
+      <c r="H13" s="15">
+        <v>8421691423220</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>19</v>
@@ -1482,13 +1494,13 @@
         <v>12345678</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="L13" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="L13" s="12" t="s">
         <v>21</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N13" s="4"/>
     </row>
@@ -1503,34 +1515,34 @@
         <v>15</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F14" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G14" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="H14" s="6">
-        <v>8421690000000</v>
+      <c r="H14" s="15">
+        <v>8421691423220</v>
       </c>
       <c r="I14" s="6" t="s">
         <v>19</v>
       </c>
       <c r="J14" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="L14" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="M14" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="K14" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="L14" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="M14" s="6" t="s">
-        <v>69</v>
       </c>
       <c r="N14" s="4"/>
     </row>
@@ -1545,34 +1557,34 @@
         <v>15</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F15" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="G15" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="H15" s="6">
-        <v>8421690000000</v>
+      <c r="H15" s="15">
+        <v>8421691423220</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>19</v>
       </c>
       <c r="J15" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="L15" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="M15" s="6" t="s">
         <v>72</v>
-      </c>
-      <c r="K15" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="L15" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="M15" s="6" t="s">
-        <v>73</v>
       </c>
       <c r="N15" s="4"/>
     </row>
@@ -1590,36 +1602,38 @@
         <v>10</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="6">
-        <v>8421690000000</v>
+      <c r="H16" s="15">
+        <v>8421691423220</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="J16" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="L16" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="L16" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="M16" s="14" t="s">
-        <v>22</v>
+      <c r="M16" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="N16" s="4"/>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A17" s="4"/>
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
       <c r="B17" s="4" t="s">
         <v>14</v>
       </c>
@@ -1630,36 +1644,38 @@
         <v>10</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="H17" s="6">
-        <v>8421690000000</v>
+        <v>79</v>
+      </c>
+      <c r="H17" s="15">
+        <v>8421691423220</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="J17" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K17" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="L17" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="M17" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="L17" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="M17" s="14" t="s">
-        <v>85</v>
-      </c>
       <c r="N17" s="4"/>
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A18" s="4"/>
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
       <c r="B18" s="4" t="s">
         <v>14</v>
       </c>
@@ -1670,37 +1686,37 @@
         <v>10</v>
       </c>
       <c r="E18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G18" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="F18" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="H18" s="6">
-        <v>8421690000000</v>
+      <c r="H18" s="15">
+        <v>8421691423220</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="J18" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="L18" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="L18" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="M18" s="14" t="s">
-        <v>91</v>
+      <c r="M18" s="11" t="s">
+        <v>89</v>
       </c>
       <c r="N18" s="4"/>
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1">
       <c r="A19" s="4">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>14</v>
@@ -1712,37 +1728,37 @@
         <v>10</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="H19" s="6">
-        <v>8421690000000</v>
+        <v>90</v>
+      </c>
+      <c r="H19" s="15">
+        <v>8421691423220</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="J19" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="L19" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="L19" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="M19" s="14" t="s">
-        <v>95</v>
+      <c r="M19" s="11" t="s">
+        <v>92</v>
       </c>
       <c r="N19" s="4"/>
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1">
       <c r="A20" s="4">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>14</v>
@@ -1754,37 +1770,37 @@
         <v>10</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="H20" s="6">
-        <v>8421690000000</v>
+        <v>93</v>
+      </c>
+      <c r="H20" s="15">
+        <v>8421691423220</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="J20" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="L20" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="L20" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="M20" s="14" t="s">
-        <v>98</v>
+      <c r="M20" s="11" t="s">
+        <v>95</v>
       </c>
       <c r="N20" s="4"/>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1">
       <c r="A21" s="4">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>14</v>
@@ -1796,37 +1812,37 @@
         <v>10</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>92</v>
+        <v>120</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="H21" s="6">
-        <v>8421690000001</v>
+        <v>93</v>
+      </c>
+      <c r="H21" s="15">
+        <v>8421691423220</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="J21" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="L21" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="L21" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="M21" s="14" t="s">
-        <v>114</v>
+      <c r="M21" s="11" t="s">
+        <v>111</v>
       </c>
       <c r="N21" s="4"/>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1">
       <c r="A22" s="4">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>14</v>
@@ -1840,12 +1856,14 @@
       <c r="E22" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="4"/>
+      <c r="F22" s="4" t="s">
+        <v>121</v>
+      </c>
       <c r="G22" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H22" s="13">
-        <v>8421690000000</v>
+      <c r="H22" s="15">
+        <v>8421691423220</v>
       </c>
       <c r="I22" s="6" t="s">
         <v>19</v>
@@ -1854,21 +1872,21 @@
         <v>20</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="L22" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="L22" s="12" t="s">
         <v>21</v>
       </c>
       <c r="M22" s="6" t="s">
-        <v>22</v>
+        <v>117</v>
       </c>
       <c r="N22" s="4"/>
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1">
       <c r="A23" s="4">
-        <v>20</v>
-      </c>
-      <c r="B23" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="4" t="s">
@@ -1878,14 +1896,16 @@
         <v>11</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="F23" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>122</v>
+      </c>
       <c r="G23" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="H23" s="13">
-        <v>8421690000000</v>
+        <v>97</v>
+      </c>
+      <c r="H23" s="15">
+        <v>8421691423220</v>
       </c>
       <c r="I23" s="6" t="s">
         <v>19</v>
@@ -1894,38 +1914,40 @@
         <v>20</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="L23" s="14" t="s">
-        <v>108</v>
+        <v>116</v>
+      </c>
+      <c r="L23" s="11" t="s">
+        <v>105</v>
       </c>
       <c r="M23" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="N23" s="4"/>
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1">
       <c r="A24" s="4">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G24" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="H24" s="13">
-        <v>8421690000000</v>
+      <c r="H24" s="15">
+        <v>8421691423220</v>
       </c>
       <c r="I24" s="6" t="s">
         <v>19</v>
@@ -1934,19 +1956,19 @@
         <v>20</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="L24" s="14" t="s">
-        <v>109</v>
+        <v>116</v>
+      </c>
+      <c r="L24" s="11" t="s">
+        <v>106</v>
       </c>
       <c r="M24" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="N24" s="4"/>
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1">
       <c r="A25" s="4">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>14</v>
@@ -1958,14 +1980,16 @@
         <v>11</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="F25" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>124</v>
+      </c>
       <c r="G25" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="H25" s="13">
-        <v>8421690000000</v>
+        <v>101</v>
+      </c>
+      <c r="H25" s="15">
+        <v>8421691423220</v>
       </c>
       <c r="I25" s="6" t="s">
         <v>19</v>
@@ -1974,19 +1998,19 @@
         <v>20</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="L25" s="14" t="s">
-        <v>110</v>
+        <v>116</v>
+      </c>
+      <c r="L25" s="11" t="s">
+        <v>107</v>
       </c>
       <c r="M25" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="N25" s="4"/>
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1">
       <c r="A26" s="4">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>14</v>
@@ -1998,14 +2022,16 @@
         <v>11</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="F26" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="G26" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="H26" s="13">
-        <v>8421690000000</v>
+        <v>103</v>
+      </c>
+      <c r="H26" s="15">
+        <v>8421691423220</v>
       </c>
       <c r="I26" s="6" t="s">
         <v>19</v>
@@ -2014,19 +2040,19 @@
         <v>20</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="L26" s="14" t="s">
-        <v>111</v>
+        <v>116</v>
+      </c>
+      <c r="L26" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="M26" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="N26" s="4"/>
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1">
       <c r="A27" s="4">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>14</v>
@@ -2038,14 +2064,16 @@
         <v>11</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="F27" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="G27" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="H27" s="13">
-        <v>8421690000001</v>
+        <v>109</v>
+      </c>
+      <c r="H27" s="15">
+        <v>8421691423220</v>
       </c>
       <c r="I27" s="6" t="s">
         <v>19</v>
@@ -2054,19 +2082,19 @@
         <v>20</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="L27" s="14" t="s">
-        <v>113</v>
+        <v>116</v>
+      </c>
+      <c r="L27" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="N27" s="12"/>
+        <v>104</v>
+      </c>
+      <c r="N27" s="10"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1">
       <c r="A28" s="4">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -2078,13 +2106,13 @@
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
-      <c r="L28" s="16"/>
+      <c r="L28" s="13"/>
       <c r="M28" s="6"/>
       <c r="N28" s="4"/>
     </row>
     <row r="29" spans="1:14" ht="15.75" customHeight="1">
       <c r="A29" s="4">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -2096,13 +2124,13 @@
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
-      <c r="L29" s="16"/>
-      <c r="M29" s="17"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="14"/>
       <c r="N29" s="4"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1">
       <c r="A30" s="4">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -2114,13 +2142,13 @@
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
-      <c r="L30" s="16"/>
+      <c r="L30" s="13"/>
       <c r="M30" s="6"/>
       <c r="N30" s="4"/>
     </row>
     <row r="31" spans="1:14" ht="15.75" customHeight="1">
       <c r="A31" s="4">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -2132,13 +2160,13 @@
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
-      <c r="L31" s="16"/>
+      <c r="L31" s="13"/>
       <c r="M31" s="6"/>
       <c r="N31" s="4"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" customHeight="1">
       <c r="A32" s="4">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -2156,7 +2184,7 @@
     </row>
     <row r="33" spans="1:14" ht="15.75" customHeight="1">
       <c r="A33" s="4">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -2174,21 +2202,21 @@
     </row>
     <row r="34" spans="1:14" ht="15.75" customHeight="1">
       <c r="A34" s="4">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
@@ -2200,21 +2228,21 @@
     </row>
     <row r="35" spans="1:14" ht="15.75" customHeight="1">
       <c r="A35" s="4">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
@@ -3356,54 +3384,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="33" customHeight="1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11"/>
-      <c r="AA1" s="11"/>
-      <c r="AB1" s="11"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="9"/>
     </row>
     <row r="2" spans="1:28" ht="15.75" customHeight="1">
       <c r="A2" s="4">
@@ -3413,25 +3441,25 @@
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="J2" s="4"/>
     </row>
@@ -4923,7 +4951,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>5</v>
@@ -4932,10 +4960,10 @@
         <v>6</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>13</v>
@@ -4946,11 +4974,11 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>

</xml_diff>

<commit_message>
UnitTest for PRODUCT_ID done and modified Excel
</commit_message>
<xml_diff>
--- a/GE3_TestCasesTemplate_2023_v1.0.xlsx
+++ b/GE3_TestCasesTemplate_2023_v1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edu/PycharmProjects/G89.2023.T20.EG3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edu\PycharmProjects\G89.2023.T20.EG3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7039B089-C12F-4948-984A-614E7FA358A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6620E71-8884-45D8-B04A-7BC908D5588C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GE3 2023 F1" sheetId="1" r:id="rId1"/>
@@ -543,21 +543,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -919,25 +919,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="116" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="116" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="30.28515625" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" customWidth="1"/>
+    <col min="1" max="2" width="10.5546875" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="30.33203125" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="31.28515625" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" customWidth="1"/>
-    <col min="13" max="13" width="70.85546875" customWidth="1"/>
-    <col min="14" max="30" width="10.5703125" customWidth="1"/>
+    <col min="10" max="10" width="31.33203125" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" customWidth="1"/>
+    <col min="13" max="13" width="70.88671875" customWidth="1"/>
+    <col min="14" max="30" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="15.75" customHeight="1">
@@ -1022,7 +1022,7 @@
       <c r="G2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="16">
         <v>8421691423220</v>
       </c>
       <c r="I2" s="6" t="s">
@@ -1034,7 +1034,7 @@
       <c r="K2" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="L2" s="13" t="s">
         <v>21</v>
       </c>
       <c r="M2" s="6" t="s">
@@ -1064,7 +1064,7 @@
       <c r="G3" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="17" t="s">
         <v>25</v>
       </c>
       <c r="I3" s="6" t="s">
@@ -1076,7 +1076,7 @@
       <c r="K3" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="L3" s="13" t="s">
         <v>21</v>
       </c>
       <c r="M3" s="6" t="s">
@@ -1106,7 +1106,7 @@
       <c r="G4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="16">
         <v>8421691423225</v>
       </c>
       <c r="I4" s="6" t="s">
@@ -1118,7 +1118,7 @@
       <c r="K4" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="L4" s="15" t="s">
+      <c r="L4" s="13" t="s">
         <v>21</v>
       </c>
       <c r="M4" s="6" t="s">
@@ -1146,13 +1146,13 @@
         <v>74</v>
       </c>
       <c r="G5" s="5"/>
-      <c r="H5" s="6"/>
+      <c r="H5" s="16"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="L5" s="15"/>
+      <c r="L5" s="13"/>
       <c r="M5" s="6"/>
       <c r="N5" s="4"/>
     </row>
@@ -1178,7 +1178,7 @@
       <c r="G6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="16">
         <v>8421691423220</v>
       </c>
       <c r="I6" s="6" t="s">
@@ -1190,7 +1190,7 @@
       <c r="K6" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="L6" s="15" t="s">
+      <c r="L6" s="13" t="s">
         <v>21</v>
       </c>
       <c r="M6" s="6" t="s">
@@ -1220,7 +1220,7 @@
       <c r="G7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="16">
         <v>8421691423220</v>
       </c>
       <c r="I7" s="6" t="s">
@@ -1232,7 +1232,7 @@
       <c r="K7" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="L7" s="15" t="s">
+      <c r="L7" s="13" t="s">
         <v>21</v>
       </c>
       <c r="M7" s="6" t="s">
@@ -1262,7 +1262,7 @@
       <c r="G8" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="16">
         <v>8421691423220</v>
       </c>
       <c r="I8" s="6" t="s">
@@ -1274,7 +1274,7 @@
       <c r="K8" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="L8" s="15" t="s">
+      <c r="L8" s="13" t="s">
         <v>21</v>
       </c>
       <c r="M8" s="6" t="s">
@@ -1304,7 +1304,7 @@
       <c r="G9" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="16">
         <v>8421691423220</v>
       </c>
       <c r="I9" s="6">
@@ -1316,7 +1316,7 @@
       <c r="K9" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="L9" s="15" t="s">
+      <c r="L9" s="13" t="s">
         <v>21</v>
       </c>
       <c r="M9" s="6" t="s">
@@ -1346,7 +1346,7 @@
       <c r="G10" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="16">
         <v>8421691423220</v>
       </c>
       <c r="I10" s="6" t="s">
@@ -1358,7 +1358,7 @@
       <c r="K10" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="L10" s="15" t="s">
+      <c r="L10" s="13" t="s">
         <v>21</v>
       </c>
       <c r="M10" s="6" t="s">
@@ -1388,8 +1388,8 @@
       <c r="G11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="6">
-        <v>8421690000000</v>
+      <c r="H11" s="16">
+        <v>8421691423220</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>19</v>
@@ -1400,7 +1400,7 @@
       <c r="K11" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="L11" s="15" t="s">
+      <c r="L11" s="13" t="s">
         <v>21</v>
       </c>
       <c r="M11" s="6" t="s">
@@ -1430,8 +1430,8 @@
       <c r="G12" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="H12" s="6">
-        <v>8421690000000</v>
+      <c r="H12" s="16">
+        <v>8421691423220</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>19</v>
@@ -1442,7 +1442,7 @@
       <c r="K12" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="L12" s="15" t="s">
+      <c r="L12" s="13" t="s">
         <v>21</v>
       </c>
       <c r="M12" s="6" t="s">
@@ -1472,8 +1472,8 @@
       <c r="G13" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="H13" s="6">
-        <v>8421690000000</v>
+      <c r="H13" s="16">
+        <v>8421691423220</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>19</v>
@@ -1484,7 +1484,7 @@
       <c r="K13" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="L13" s="15" t="s">
+      <c r="L13" s="13" t="s">
         <v>21</v>
       </c>
       <c r="M13" s="6" t="s">
@@ -1514,8 +1514,8 @@
       <c r="G14" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="H14" s="6">
-        <v>8421690000000</v>
+      <c r="H14" s="16">
+        <v>8421691423220</v>
       </c>
       <c r="I14" s="6" t="s">
         <v>19</v>
@@ -1526,7 +1526,7 @@
       <c r="K14" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="L14" s="15" t="s">
+      <c r="L14" s="13" t="s">
         <v>21</v>
       </c>
       <c r="M14" s="6" t="s">
@@ -1556,8 +1556,8 @@
       <c r="G15" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="H15" s="6">
-        <v>8421690000000</v>
+      <c r="H15" s="16">
+        <v>8421691423220</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>19</v>
@@ -1568,7 +1568,7 @@
       <c r="K15" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="L15" s="15" t="s">
+      <c r="L15" s="13" t="s">
         <v>21</v>
       </c>
       <c r="M15" s="6" t="s">
@@ -1598,8 +1598,8 @@
       <c r="G16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="6">
-        <v>8421690000000</v>
+      <c r="H16" s="16">
+        <v>8421691423220</v>
       </c>
       <c r="I16" s="6" t="s">
         <v>51</v>
@@ -1610,10 +1610,10 @@
       <c r="K16" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="L16" s="15" t="s">
+      <c r="L16" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="M16" s="14" t="s">
+      <c r="M16" s="12" t="s">
         <v>22</v>
       </c>
       <c r="N16" s="4"/>
@@ -1638,8 +1638,8 @@
       <c r="G17" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="H17" s="6">
-        <v>8421690000000</v>
+      <c r="H17" s="16">
+        <v>8421691423220</v>
       </c>
       <c r="I17" s="6" t="s">
         <v>51</v>
@@ -1650,10 +1650,10 @@
       <c r="K17" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="L17" s="15" t="s">
+      <c r="L17" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="M17" s="14" t="s">
+      <c r="M17" s="12" t="s">
         <v>85</v>
       </c>
       <c r="N17" s="4"/>
@@ -1678,8 +1678,8 @@
       <c r="G18" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="H18" s="6">
-        <v>8421690000000</v>
+      <c r="H18" s="16">
+        <v>8421691423220</v>
       </c>
       <c r="I18" s="6" t="s">
         <v>51</v>
@@ -1690,10 +1690,10 @@
       <c r="K18" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="L18" s="15" t="s">
+      <c r="L18" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="M18" s="14" t="s">
+      <c r="M18" s="12" t="s">
         <v>91</v>
       </c>
       <c r="N18" s="4"/>
@@ -1720,8 +1720,8 @@
       <c r="G19" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="H19" s="6">
-        <v>8421690000000</v>
+      <c r="H19" s="16">
+        <v>8421691423220</v>
       </c>
       <c r="I19" s="6" t="s">
         <v>51</v>
@@ -1732,10 +1732,10 @@
       <c r="K19" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="L19" s="15" t="s">
+      <c r="L19" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="M19" s="14" t="s">
+      <c r="M19" s="12" t="s">
         <v>95</v>
       </c>
       <c r="N19" s="4"/>
@@ -1762,8 +1762,8 @@
       <c r="G20" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="H20" s="6">
-        <v>8421690000000</v>
+      <c r="H20" s="16">
+        <v>8421691423220</v>
       </c>
       <c r="I20" s="6" t="s">
         <v>51</v>
@@ -1774,10 +1774,10 @@
       <c r="K20" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="L20" s="15" t="s">
+      <c r="L20" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="M20" s="14" t="s">
+      <c r="M20" s="12" t="s">
         <v>98</v>
       </c>
       <c r="N20" s="4"/>
@@ -1804,8 +1804,8 @@
       <c r="G21" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="H21" s="6">
-        <v>8421690000001</v>
+      <c r="H21" s="16">
+        <v>8421691423220</v>
       </c>
       <c r="I21" s="6" t="s">
         <v>51</v>
@@ -1816,10 +1816,10 @@
       <c r="K21" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="L21" s="15" t="s">
+      <c r="L21" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="M21" s="14" t="s">
+      <c r="M21" s="12" t="s">
         <v>114</v>
       </c>
       <c r="N21" s="4"/>
@@ -1844,8 +1844,8 @@
       <c r="G22" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H22" s="13">
-        <v>8421690000000</v>
+      <c r="H22" s="16">
+        <v>8421691423220</v>
       </c>
       <c r="I22" s="6" t="s">
         <v>19</v>
@@ -1856,7 +1856,7 @@
       <c r="K22" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="L22" s="15" t="s">
+      <c r="L22" s="13" t="s">
         <v>21</v>
       </c>
       <c r="M22" s="6" t="s">
@@ -1868,7 +1868,7 @@
       <c r="A23" s="4">
         <v>20</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="4" t="s">
@@ -1884,8 +1884,8 @@
       <c r="G23" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="H23" s="13">
-        <v>8421690000000</v>
+      <c r="H23" s="16">
+        <v>8421691423220</v>
       </c>
       <c r="I23" s="6" t="s">
         <v>19</v>
@@ -1896,7 +1896,7 @@
       <c r="K23" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="L23" s="14" t="s">
+      <c r="L23" s="12" t="s">
         <v>108</v>
       </c>
       <c r="M23" s="6" t="s">
@@ -1911,21 +1911,21 @@
       <c r="B24" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="8" t="s">
+      <c r="F24" s="8"/>
+      <c r="G24" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="H24" s="13">
-        <v>8421690000000</v>
+      <c r="H24" s="16">
+        <v>8421691423220</v>
       </c>
       <c r="I24" s="6" t="s">
         <v>19</v>
@@ -1936,7 +1936,7 @@
       <c r="K24" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="L24" s="14" t="s">
+      <c r="L24" s="12" t="s">
         <v>109</v>
       </c>
       <c r="M24" s="6" t="s">
@@ -1964,8 +1964,8 @@
       <c r="G25" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="H25" s="13">
-        <v>8421690000000</v>
+      <c r="H25" s="16">
+        <v>8421691423220</v>
       </c>
       <c r="I25" s="6" t="s">
         <v>19</v>
@@ -1976,7 +1976,7 @@
       <c r="K25" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="L25" s="14" t="s">
+      <c r="L25" s="12" t="s">
         <v>110</v>
       </c>
       <c r="M25" s="6" t="s">
@@ -2004,8 +2004,8 @@
       <c r="G26" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="H26" s="13">
-        <v>8421690000000</v>
+      <c r="H26" s="16">
+        <v>8421691423220</v>
       </c>
       <c r="I26" s="6" t="s">
         <v>19</v>
@@ -2016,7 +2016,7 @@
       <c r="K26" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="L26" s="14" t="s">
+      <c r="L26" s="12" t="s">
         <v>111</v>
       </c>
       <c r="M26" s="6" t="s">
@@ -2044,8 +2044,8 @@
       <c r="G27" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="H27" s="13">
-        <v>8421690000001</v>
+      <c r="H27" s="16">
+        <v>8421691423220</v>
       </c>
       <c r="I27" s="6" t="s">
         <v>19</v>
@@ -2056,13 +2056,13 @@
       <c r="K27" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="L27" s="14" t="s">
+      <c r="L27" s="12" t="s">
         <v>113</v>
       </c>
       <c r="M27" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="N27" s="12"/>
+      <c r="N27" s="11"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1">
       <c r="A28" s="4">
@@ -2078,7 +2078,7 @@
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
-      <c r="L28" s="16"/>
+      <c r="L28" s="14"/>
       <c r="M28" s="6"/>
       <c r="N28" s="4"/>
     </row>
@@ -2096,8 +2096,8 @@
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
-      <c r="L29" s="16"/>
-      <c r="M29" s="17"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="15"/>
       <c r="N29" s="4"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1">
@@ -2114,7 +2114,7 @@
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
-      <c r="L30" s="16"/>
+      <c r="L30" s="14"/>
       <c r="M30" s="6"/>
       <c r="N30" s="4"/>
     </row>
@@ -2132,7 +2132,7 @@
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
-      <c r="L31" s="16"/>
+      <c r="L31" s="14"/>
       <c r="M31" s="6"/>
       <c r="N31" s="4"/>
     </row>
@@ -3342,68 +3342,68 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" customWidth="1"/>
-    <col min="4" max="4" width="44.140625" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
-    <col min="6" max="6" width="62.28515625" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" customWidth="1"/>
-    <col min="8" max="8" width="36.7109375" customWidth="1"/>
-    <col min="9" max="10" width="33.7109375" customWidth="1"/>
-    <col min="11" max="28" width="10.5703125" customWidth="1"/>
+    <col min="1" max="2" width="10.5546875" customWidth="1"/>
+    <col min="3" max="3" width="26.5546875" customWidth="1"/>
+    <col min="4" max="4" width="44.109375" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" customWidth="1"/>
+    <col min="6" max="6" width="62.33203125" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" customWidth="1"/>
+    <col min="8" max="8" width="36.6640625" customWidth="1"/>
+    <col min="9" max="10" width="33.6640625" customWidth="1"/>
+    <col min="11" max="28" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="33" customHeight="1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11"/>
-      <c r="AA1" s="11"/>
-      <c r="AB1" s="11"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
+      <c r="AA1" s="10"/>
+      <c r="AB1" s="10"/>
     </row>
     <row r="2" spans="1:28" ht="15.75" customHeight="1">
       <c r="A2" s="4">
@@ -4907,15 +4907,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="62.28515625" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" customWidth="1"/>
-    <col min="6" max="7" width="33.7109375" customWidth="1"/>
-    <col min="8" max="25" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="62.33203125" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" customWidth="1"/>
+    <col min="6" max="7" width="33.6640625" customWidth="1"/>
+    <col min="8" max="25" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Added Product_ID length related tests
</commit_message>
<xml_diff>
--- a/GE3_TestCasesTemplate_2023_v1.0.xlsx
+++ b/GE3_TestCasesTemplate_2023_v1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edu\PycharmProjects\G89.2023.T20.EG3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6620E71-8884-45D8-B04A-7BC908D5588C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B2E48E-0A0C-457A-B402-F18CB2687F00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="1515" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GE3 2023 F1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="125">
   <si>
     <t>#</t>
   </si>
@@ -108,9 +108,6 @@
   </si>
   <si>
     <t>"PREMIUM"</t>
-  </si>
-  <si>
-    <t>Exception: Product Id not valid</t>
   </si>
   <si>
     <t>CE_NV_3</t>
@@ -256,9 +253,6 @@
     <t>Exception: Address too long</t>
   </si>
   <si>
-    <t>CE_NV_4</t>
-  </si>
-  <si>
     <t>CE_NV_8</t>
   </si>
   <si>
@@ -392,6 +386,27 @@
   </si>
   <si>
     <t>"654314159"</t>
+  </si>
+  <si>
+    <t>PRODUCT ID TOO SHORT</t>
+  </si>
+  <si>
+    <t>PRODUCT ID TOO LONG</t>
+  </si>
+  <si>
+    <t>Exception: Product Id not valid, not an EAN13 code</t>
+  </si>
+  <si>
+    <t>Exception: Product Id not valid, id too short</t>
+  </si>
+  <si>
+    <t>Exception: Product Id not valid, id too long</t>
+  </si>
+  <si>
+    <t>Exception: Product Id not valid, id must be numeric</t>
+  </si>
+  <si>
+    <t>e01521684a7f9535e9fa098a2b86565f</t>
   </si>
 </sst>
 </file>
@@ -665,7 +680,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:N44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:N45">
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="#"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="I/O"/>
@@ -917,10 +932,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD1001"/>
+  <dimension ref="A1:AD1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="116" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="15" customHeight="1"/>
@@ -931,7 +946,7 @@
     <col min="5" max="5" width="11.33203125" customWidth="1"/>
     <col min="6" max="6" width="14.6640625" customWidth="1"/>
     <col min="7" max="7" width="30.33203125" customWidth="1"/>
-    <col min="8" max="8" width="18.109375" customWidth="1"/>
+    <col min="8" max="8" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
     <col min="10" max="10" width="31.33203125" customWidth="1"/>
     <col min="11" max="11" width="14.33203125" customWidth="1"/>
@@ -1032,13 +1047,13 @@
         <v>20</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L2" s="13" t="s">
         <v>21</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>22</v>
+        <v>124</v>
       </c>
       <c r="N2" s="4"/>
     </row>
@@ -1062,7 +1077,7 @@
         <v>24</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H3" s="17" t="s">
         <v>25</v>
@@ -1074,13 +1089,13 @@
         <v>20</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L3" s="13" t="s">
         <v>21</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>27</v>
+        <v>123</v>
       </c>
       <c r="N3" s="4"/>
     </row>
@@ -1101,10 +1116,10 @@
         <v>23</v>
       </c>
       <c r="F4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="H4" s="16">
         <v>8421691423225</v>
@@ -1116,13 +1131,13 @@
         <v>20</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L4" s="13" t="s">
         <v>21</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>27</v>
+        <v>120</v>
       </c>
       <c r="N4" s="4"/>
     </row>
@@ -1142,18 +1157,28 @@
       <c r="E5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H5" s="16">
+        <v>8421691</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="K5" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="L5" s="13"/>
-      <c r="M5" s="6"/>
+        <v>117</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>121</v>
+      </c>
       <c r="N5" s="4"/>
     </row>
     <row r="6" spans="1:30" ht="15.75" customHeight="1">
@@ -1170,31 +1195,29 @@
         <v>7</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>78</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="F6" s="5"/>
       <c r="G6" s="5" t="s">
-        <v>18</v>
+        <v>119</v>
       </c>
       <c r="H6" s="16">
-        <v>8421691423220</v>
+        <v>8421691423220150</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L6" s="13" t="s">
         <v>21</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="N6" s="4"/>
     </row>
@@ -1209,13 +1232,13 @@
         <v>15</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>16</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>18</v>
@@ -1224,13 +1247,13 @@
         <v>8421691423220</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L7" s="13" t="s">
         <v>21</v>
@@ -1251,34 +1274,34 @@
         <v>15</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>81</v>
+        <v>18</v>
       </c>
       <c r="H8" s="16">
         <v>8421691423220</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L8" s="13" t="s">
         <v>21</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>116</v>
+        <v>22</v>
       </c>
       <c r="N8" s="4"/>
     </row>
@@ -1293,34 +1316,34 @@
         <v>15</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>23</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="H9" s="16">
         <v>8421691423220</v>
       </c>
-      <c r="I9" s="6">
-        <v>123</v>
+      <c r="I9" s="6" t="s">
+        <v>52</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L9" s="13" t="s">
         <v>21</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="N9" s="4"/>
     </row>
@@ -1335,34 +1358,34 @@
         <v>15</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>23</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="H10" s="16">
         <v>8421691423220</v>
       </c>
-      <c r="I10" s="6" t="s">
-        <v>55</v>
+      <c r="I10" s="6">
+        <v>123</v>
       </c>
       <c r="J10" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L10" s="13" t="s">
         <v>21</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="N10" s="4"/>
     </row>
@@ -1377,34 +1400,34 @@
         <v>15</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="H11" s="16">
         <v>8421691423220</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L11" s="13" t="s">
         <v>21</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>22</v>
+        <v>116</v>
       </c>
       <c r="N11" s="4"/>
     </row>
@@ -1419,16 +1442,16 @@
         <v>15</v>
       </c>
       <c r="D12" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="G12" s="5" t="s">
-        <v>60</v>
+        <v>18</v>
       </c>
       <c r="H12" s="16">
         <v>8421691423220</v>
@@ -1437,16 +1460,16 @@
         <v>19</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>61</v>
+        <v>20</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L12" s="13" t="s">
         <v>21</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
       <c r="N12" s="4"/>
     </row>
@@ -1461,16 +1484,16 @@
         <v>15</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>23</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H13" s="16">
         <v>8421691423220</v>
@@ -1478,17 +1501,17 @@
       <c r="I13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="6">
-        <v>12345678</v>
+      <c r="J13" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L13" s="13" t="s">
         <v>21</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="N13" s="4"/>
     </row>
@@ -1503,16 +1526,16 @@
         <v>15</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>23</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H14" s="16">
         <v>8421691423220</v>
@@ -1520,17 +1543,17 @@
       <c r="I14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="6" t="s">
-        <v>68</v>
+      <c r="J14" s="6">
+        <v>12345678</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L14" s="13" t="s">
         <v>21</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="N14" s="4"/>
     </row>
@@ -1545,16 +1568,16 @@
         <v>15</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>23</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H15" s="16">
         <v>8421691423220</v>
@@ -1563,16 +1586,16 @@
         <v>19</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L15" s="13" t="s">
         <v>21</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="N15" s="4"/>
     </row>
@@ -1580,46 +1603,48 @@
       <c r="A16" s="4">
         <v>15</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="4" t="s">
+      <c r="D16" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>18</v>
+      <c r="F16" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="H16" s="16">
         <v>8421691423220</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L16" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="M16" s="12" t="s">
-        <v>22</v>
+      <c r="M16" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="N16" s="4"/>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A17" s="4"/>
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
       <c r="B17" s="4" t="s">
         <v>14</v>
       </c>
@@ -1633,33 +1658,35 @@
         <v>23</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>80</v>
+        <v>18</v>
       </c>
       <c r="H17" s="16">
         <v>8421691423220</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J17" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>84</v>
+        <v>117</v>
       </c>
       <c r="L17" s="13" t="s">
         <v>21</v>
       </c>
       <c r="M17" s="12" t="s">
-        <v>85</v>
+        <v>22</v>
       </c>
       <c r="N17" s="4"/>
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A18" s="4"/>
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
       <c r="B18" s="4" t="s">
         <v>14</v>
       </c>
@@ -1670,37 +1697,37 @@
         <v>10</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>88</v>
+        <v>23</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H18" s="16">
         <v>8421691423220</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J18" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="L18" s="13" t="s">
         <v>21</v>
       </c>
       <c r="M18" s="12" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="N18" s="4"/>
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1">
       <c r="A19" s="4">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>14</v>
@@ -1712,37 +1739,37 @@
         <v>10</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="H19" s="16">
         <v>8421691423220</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J19" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="L19" s="13" t="s">
         <v>21</v>
       </c>
       <c r="M19" s="12" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="N19" s="4"/>
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1">
       <c r="A20" s="4">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>14</v>
@@ -1757,34 +1784,34 @@
         <v>23</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H20" s="16">
         <v>8421691423220</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J20" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="L20" s="13" t="s">
         <v>21</v>
       </c>
       <c r="M20" s="12" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="N20" s="4"/>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1">
       <c r="A21" s="4">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>14</v>
@@ -1799,34 +1826,34 @@
         <v>23</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H21" s="16">
         <v>8421691423220</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J21" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="L21" s="13" t="s">
         <v>21</v>
       </c>
       <c r="M21" s="12" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="N21" s="4"/>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1">
       <c r="A22" s="4">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>14</v>
@@ -1835,40 +1862,42 @@
         <v>15</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="G22" s="4" t="s">
-        <v>18</v>
+        <v>94</v>
       </c>
       <c r="H22" s="16">
         <v>8421691423220</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="J22" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="L22" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="M22" s="6" t="s">
-        <v>22</v>
+      <c r="M22" s="12" t="s">
+        <v>112</v>
       </c>
       <c r="N22" s="4"/>
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1">
       <c r="A23" s="4">
-        <v>20</v>
-      </c>
-      <c r="B23" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="4" t="s">
@@ -1878,11 +1907,11 @@
         <v>11</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4" t="s">
-        <v>100</v>
+        <v>18</v>
       </c>
       <c r="H23" s="16">
         <v>8421691423220</v>
@@ -1894,35 +1923,35 @@
         <v>20</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="L23" s="12" t="s">
-        <v>108</v>
+        <v>117</v>
+      </c>
+      <c r="L23" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="M23" s="6" t="s">
-        <v>101</v>
+        <v>22</v>
       </c>
       <c r="N23" s="4"/>
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1">
       <c r="A24" s="4">
-        <v>21</v>
-      </c>
-      <c r="B24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E24" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="F24" s="8"/>
-      <c r="G24" s="7" t="s">
-        <v>102</v>
+      <c r="E24" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4" t="s">
+        <v>98</v>
       </c>
       <c r="H24" s="16">
         <v>8421691423220</v>
@@ -1934,35 +1963,35 @@
         <v>20</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L24" s="12" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="M24" s="6" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="N24" s="4"/>
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1">
       <c r="A25" s="4">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4" t="s">
-        <v>104</v>
+      <c r="E25" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F25" s="8"/>
+      <c r="G25" s="7" t="s">
+        <v>100</v>
       </c>
       <c r="H25" s="16">
         <v>8421691423220</v>
@@ -1974,19 +2003,19 @@
         <v>20</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L25" s="12" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="M25" s="6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="N25" s="4"/>
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1">
       <c r="A26" s="4">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>14</v>
@@ -1998,11 +2027,11 @@
         <v>11</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="H26" s="16">
         <v>8421691423220</v>
@@ -2014,19 +2043,19 @@
         <v>20</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L26" s="12" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="M26" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="N26" s="4"/>
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1">
       <c r="A27" s="4">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>14</v>
@@ -2038,11 +2067,11 @@
         <v>11</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="4" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="H27" s="16">
         <v>8421691423220</v>
@@ -2054,37 +2083,59 @@
         <v>20</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L27" s="12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="N27" s="11"/>
+        <v>105</v>
+      </c>
+      <c r="N27" s="4"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1">
       <c r="A28" s="4">
-        <v>25</v>
-      </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="6"/>
-      <c r="N28" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="H28" s="16">
+        <v>8421691423220</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K28" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="L28" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="M28" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="N28" s="11"/>
     </row>
     <row r="29" spans="1:14" ht="15.75" customHeight="1">
       <c r="A29" s="4">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -2097,12 +2148,12 @@
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
       <c r="L29" s="14"/>
-      <c r="M29" s="15"/>
+      <c r="M29" s="6"/>
       <c r="N29" s="4"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1">
       <c r="A30" s="4">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -2115,19 +2166,19 @@
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
       <c r="L30" s="14"/>
-      <c r="M30" s="6"/>
+      <c r="M30" s="15"/>
       <c r="N30" s="4"/>
     </row>
     <row r="31" spans="1:14" ht="15.75" customHeight="1">
       <c r="A31" s="4">
-        <v>28</v>
-      </c>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
@@ -2138,7 +2189,7 @@
     </row>
     <row r="32" spans="1:14" ht="15.75" customHeight="1">
       <c r="A32" s="4">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -2146,17 +2197,17 @@
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="6"/>
       <c r="N32" s="4"/>
     </row>
     <row r="33" spans="1:14" ht="15.75" customHeight="1">
       <c r="A33" s="4">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -2173,23 +2224,12 @@
       <c r="N33" s="4"/>
     </row>
     <row r="34" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A34" s="4">
-        <v>31</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
       <c r="D34" s="4"/>
-      <c r="E34" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="E34" s="4"/>
       <c r="F34" s="4"/>
-      <c r="G34" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
@@ -2199,22 +2239,19 @@
       <c r="N34" s="4"/>
     </row>
     <row r="35" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A35" s="4">
-        <v>32</v>
-      </c>
       <c r="B35" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
@@ -2225,13 +2262,20 @@
       <c r="N35" s="4"/>
     </row>
     <row r="36" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
+      <c r="B36" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
+      <c r="E36" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
+      <c r="G36" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
@@ -2368,7 +2412,22 @@
       <c r="M44" s="4"/>
       <c r="N44" s="4"/>
     </row>
-    <row r="45" spans="1:14" ht="15.75" customHeight="1"/>
+    <row r="45" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="4"/>
+      <c r="L45" s="4"/>
+      <c r="M45" s="4"/>
+      <c r="N45" s="4"/>
+    </row>
     <row r="46" spans="1:14" ht="15.75" customHeight="1"/>
     <row r="47" spans="1:14" ht="15.75" customHeight="1"/>
     <row r="48" spans="1:14" ht="15.75" customHeight="1"/>
@@ -3325,6 +3384,7 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
     <row r="1001" ht="15.75" customHeight="1"/>
+    <row r="1002" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -3360,13 +3420,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>36</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>37</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>5</v>
@@ -3375,13 +3435,13 @@
         <v>6</v>
       </c>
       <c r="G1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>39</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>40</v>
       </c>
       <c r="J1" s="9" t="s">
         <v>13</v>
@@ -3413,25 +3473,25 @@
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="J2" s="4"/>
     </row>
@@ -4923,7 +4983,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>5</v>
@@ -4932,10 +4992,10 @@
         <v>6</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>13</v>
@@ -4946,11 +5006,11 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>

</xml_diff>